<commit_message>
2018-01-09: 1. finsh add_friend & user_friend_group and test case; 2. ready to change rule format(add range and change require format)
</commit_message>
<xml_diff>
--- a/doc/POST参数/post参数.xlsx
+++ b/doc/POST参数/post参数.xlsx
@@ -91,6 +91,43 @@
         </r>
       </text>
     </comment>
+    <comment ref="H3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>ZHANG Wei AG:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+{
+      fieldName1:
+          {
+                from:
+                to:
+                eleArray
+          },
+      fieldName2:
+          {
+                from:
+                to:
+                eleArray
+          },
+}</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="F4" authorId="1" shapeId="0">
       <text>
         <r>
@@ -280,13 +317,6 @@
     </r>
   </si>
   <si>
-    <t>用于字段值为array或者mixed操作，对其中的元素进行添加/删除/移动（使用edit，而不是update，防止混淆）
-fieldName:{from: eleArray中元素，原始位于哪个记录，如果没有（不是null或者undefined，而是没有key），说明是添加
- to: eleArray中元素，要移动到哪个记录，如果没有，说明是删除
- eleArray:要操作的记录。可以为空数组
-}</t>
-  </si>
-  <si>
     <t>当前暂时用于记录群事件。
 包括几个子字段：
 1. eventId--id含义定义在js文件中，减少db的查询
@@ -521,12 +551,20 @@
     <t>editSubField(对象)</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
+  <si>
+    <t>用于字段值为array或者mixed操作，对其中的元素进行添加/删除/移动（使用edit，而不是update，防止混淆）
+fieldName:{from: eleArray中元素，原始位于哪个记录，如果没有（不是null或者undefined，而是没有key），说明是添加
+ to: eleArray中元素，要移动到哪个记录，如果没有，说明是删除
+ eleArray:要操作的记录。可以为空数组
+}</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -573,6 +611,19 @@
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -926,7 +977,7 @@
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
@@ -963,7 +1014,7 @@
         <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I1" t="s">
         <v>6</v>
@@ -1033,10 +1084,10 @@
         <v>13</v>
       </c>
       <c r="H3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>15</v>
@@ -1047,7 +1098,7 @@
     </row>
     <row r="4" spans="1:11" ht="56.5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>13</v>
@@ -1062,7 +1113,7 @@
         <v>13</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>13</v>
@@ -1082,7 +1133,7 @@
     </row>
     <row r="5" spans="1:11" ht="42" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>13</v>
@@ -1091,13 +1142,13 @@
         <v>11</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>13</v>
@@ -1117,7 +1168,7 @@
     </row>
     <row r="6" spans="1:11" ht="143" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>13</v>
@@ -1135,21 +1186,21 @@
         <v>13</v>
       </c>
       <c r="G6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K6" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>

</xml_diff>

<commit_message>
2018-01-30: 1. server side api almost done
</commit_message>
<xml_diff>
--- a/doc/POST参数/post参数.xlsx
+++ b/doc/POST参数/post参数.xlsx
@@ -91,6 +91,33 @@
         </r>
       </text>
     </comment>
+    <comment ref="K1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">ZHANG Wei AG:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>对array进行操作
+field:{add:[id1],remove:[id2]}</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="H3" authorId="0" shapeId="0">
       <text>
         <r>
@@ -150,7 +177,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K6" authorId="0" shapeId="0">
+    <comment ref="L6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -185,7 +212,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="32">
   <si>
     <t>recordInfo</t>
   </si>
@@ -559,12 +586,16 @@
 }</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
+  <si>
+    <t>manipulateArray</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -624,6 +655,14 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -974,27 +1013,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.26953125" customWidth="1"/>
     <col min="2" max="2" width="45.36328125" customWidth="1"/>
-    <col min="3" max="3" width="12.6328125" customWidth="1"/>
+    <col min="3" max="3" width="12.6328125" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="19.90625" customWidth="1"/>
     <col min="5" max="5" width="11.453125" customWidth="1"/>
     <col min="6" max="6" width="43.6328125" customWidth="1"/>
     <col min="7" max="7" width="23.90625" customWidth="1"/>
     <col min="8" max="8" width="57.08984375" customWidth="1"/>
     <col min="9" max="9" width="54.36328125" customWidth="1"/>
-    <col min="10" max="10" width="17.90625" customWidth="1"/>
+    <col min="10" max="11" width="17.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1022,11 +1061,14 @@
       <c r="J1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="L1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="64" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="64" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1057,11 +1099,14 @@
       <c r="J2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="112" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="112" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -1092,11 +1137,14 @@
       <c r="J3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="56.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="56.5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -1127,11 +1175,14 @@
       <c r="J4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="42" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="42" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -1162,11 +1213,14 @@
       <c r="J5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L5">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="143" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="143" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -1194,11 +1248,11 @@
       <c r="I6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="L6" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>28</v>
       </c>
@@ -1215,8 +1269,8 @@
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
2018-02-02: almost done, interact with client
</commit_message>
<xml_diff>
--- a/doc/POST参数/post参数.xlsx
+++ b/doc/POST参数/post参数.xlsx
@@ -91,6 +91,33 @@
         </r>
       </text>
     </comment>
+    <comment ref="K1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">ZHANG Wei AG:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>对array进行操作
+field:{add:[id1],remove:[id2]}</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="H3" authorId="0" shapeId="0">
       <text>
         <r>
@@ -150,7 +177,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K6" authorId="0" shapeId="0">
+    <comment ref="L6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -185,7 +212,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="32">
   <si>
     <t>recordInfo</t>
   </si>
@@ -559,12 +586,16 @@
 }</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
+  <si>
+    <t>manipulateArray</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -624,6 +655,14 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -974,27 +1013,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.26953125" customWidth="1"/>
     <col min="2" max="2" width="45.36328125" customWidth="1"/>
-    <col min="3" max="3" width="12.6328125" customWidth="1"/>
+    <col min="3" max="3" width="12.6328125" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="19.90625" customWidth="1"/>
     <col min="5" max="5" width="11.453125" customWidth="1"/>
     <col min="6" max="6" width="43.6328125" customWidth="1"/>
     <col min="7" max="7" width="23.90625" customWidth="1"/>
     <col min="8" max="8" width="57.08984375" customWidth="1"/>
     <col min="9" max="9" width="54.36328125" customWidth="1"/>
-    <col min="10" max="10" width="17.90625" customWidth="1"/>
+    <col min="10" max="11" width="17.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1022,11 +1061,14 @@
       <c r="J1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="L1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="64" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="64" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1057,11 +1099,14 @@
       <c r="J2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="112" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="112" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -1092,11 +1137,14 @@
       <c r="J3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="56.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="56.5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -1127,11 +1175,14 @@
       <c r="J4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="42" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="42" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -1162,11 +1213,14 @@
       <c r="J5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L5">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="143" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="143" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -1194,11 +1248,11 @@
       <c r="I6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="L6" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>28</v>
       </c>
@@ -1215,8 +1269,8 @@
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
2018-02-09: add client related file generate function
</commit_message>
<xml_diff>
--- a/doc/POST参数/post参数.xlsx
+++ b/doc/POST参数/post参数.xlsx
@@ -91,6 +91,33 @@
         </r>
       </text>
     </comment>
+    <comment ref="K1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">ZHANG Wei AG:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>对array进行操作
+field:{add:[id1],remove:[id2]}</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="H3" authorId="0" shapeId="0">
       <text>
         <r>
@@ -150,7 +177,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K6" authorId="0" shapeId="0">
+    <comment ref="L6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -185,7 +212,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="32">
   <si>
     <t>recordInfo</t>
   </si>
@@ -559,12 +586,16 @@
 }</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
+  <si>
+    <t>manipulateArray</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -624,6 +655,14 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -974,27 +1013,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.26953125" customWidth="1"/>
     <col min="2" max="2" width="45.36328125" customWidth="1"/>
-    <col min="3" max="3" width="12.6328125" customWidth="1"/>
+    <col min="3" max="3" width="12.6328125" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="19.90625" customWidth="1"/>
     <col min="5" max="5" width="11.453125" customWidth="1"/>
     <col min="6" max="6" width="43.6328125" customWidth="1"/>
     <col min="7" max="7" width="23.90625" customWidth="1"/>
     <col min="8" max="8" width="57.08984375" customWidth="1"/>
     <col min="9" max="9" width="54.36328125" customWidth="1"/>
-    <col min="10" max="10" width="17.90625" customWidth="1"/>
+    <col min="10" max="11" width="17.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1022,11 +1061,14 @@
       <c r="J1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="L1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="64" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="64" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1057,11 +1099,14 @@
       <c r="J2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="112" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="112" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -1092,11 +1137,14 @@
       <c r="J3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="56.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="56.5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -1127,11 +1175,14 @@
       <c r="J4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="42" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="42" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -1162,11 +1213,14 @@
       <c r="J5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L5">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="143" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="143" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -1194,11 +1248,11 @@
       <c r="I6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="L6" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>28</v>
       </c>
@@ -1215,8 +1269,8 @@
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
2018-04-01: 1. new structure to route and handle request(now only in user); 2. other
</commit_message>
<xml_diff>
--- a/doc/POST参数/post参数.xlsx
+++ b/doc/POST参数/post参数.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24140" windowHeight="12630"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="24140" windowHeight="12630"/>
   </bookViews>
   <sheets>
     <sheet name="part" sheetId="1" r:id="rId1"/>
@@ -51,6 +51,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>对单个字段进行检查（例如检查用户唯一性已经密码的正确性
@@ -68,6 +69,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>验证格式
@@ -85,6 +87,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>验证单个值</t>
@@ -115,6 +118,112 @@
           </rPr>
           <t>对array进行操作
 field:{add:[id1],remove:[id2]}</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>ZHANG Wei AG:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+1. </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>可以用在任何method。
+2.格式简单，直接通过validateValue验证</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>ZHANG Wei AG:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>同captcha
+1. 适用任何method
+2. 直接通过validateVlaue验证</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>ZHANG Wei AG:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>格式简单，validateFormat中检查是否为数组，validateVlaue中检查是否为dataUrl（正则）
+Size散落在其他函数中检查</t>
         </r>
       </text>
     </comment>
@@ -162,6 +271,7 @@
             <b/>
             <sz val="9"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>Ada:</t>
@@ -170,6 +280,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
@@ -201,6 +312,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>判断输入记录是否和db中存储的一直（例如登录）</t>
@@ -212,7 +324,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="35">
   <si>
     <t>recordInfo</t>
   </si>
@@ -266,6 +378,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>创建之后返回第一页</t>
@@ -290,6 +403,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>创建之后所有条件归零（防止新建数据无法显示）</t>
@@ -317,6 +431,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>update之后不改变页数</t>
@@ -338,6 +453,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>理由同上</t>
@@ -370,6 +486,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>，选择全部记率</t>
@@ -405,6 +522,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>删除以后，需要把后续的记录补上</t>
@@ -426,6 +544,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>补上记录的条件</t>
@@ -450,6 +569,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
@@ -470,6 +590,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>因为过滤字段值只考虑</t>
@@ -488,6 +609,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>操作，所以无需</t>
@@ -507,6 +629,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>如果值为空</t>
@@ -525,6 +648,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>，则返回所有记录；如果超出</t>
@@ -543,6 +667,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>，则不查</t>
@@ -561,6 +686,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>，直接返回空数组</t>
@@ -590,12 +716,24 @@
     <t>manipulateArray</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
+  <si>
+    <t>captcha</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>sms</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>dataUrl</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -613,6 +751,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
@@ -629,17 +768,20 @@
     <font>
       <sz val="9"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="9"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -664,6 +806,21 @@
       <family val="3"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -687,7 +844,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -701,6 +858,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1013,10 +1173,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
@@ -1033,7 +1193,7 @@
     <col min="10" max="11" width="17.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1067,8 +1227,17 @@
       <c r="L1" t="s">
         <v>8</v>
       </c>
+      <c r="M1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" ht="64" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="64" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1106,7 +1275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="112" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="112" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -1144,7 +1313,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="56.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="56.5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -1182,7 +1351,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="42" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="42" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -1220,7 +1389,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="143" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="143" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -1252,16 +1421,16 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+    <row r="9" spans="1:15" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
2018-12-14: 1. part choose_friend done;2. send recommend with choose_friend done
</commit_message>
<xml_diff>
--- a/doc/POST参数/post参数.xlsx
+++ b/doc/POST参数/post参数.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ss_vue_express\doc\POST参数\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\U\ss_vue_express\doc\POST参数\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,6 +24,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>ZHANG Wei AG</author>
+    <author>Administrator</author>
     <author>Ada</author>
   </authors>
   <commentList>
@@ -224,6 +225,31 @@
           </rPr>
           <t>格式简单，validateFormat中检查是否为数组，validateVlaue中检查是否为dataUrl（正则）
 Size散落在其他函数中检查</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P1" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Administrator:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+1. 采用post/put方法上传
+2. 和CRUD无联系（不是create/update/delete/get），只是用来传递选择好友的信息</t>
         </r>
       </text>
     </comment>
@@ -264,7 +290,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F4" authorId="1" shapeId="0">
+    <comment ref="F4" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -324,7 +350,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="36">
   <si>
     <t>recordInfo</t>
   </si>
@@ -705,39 +731,41 @@
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
+    <t>manipulateArray</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>captcha</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>sms</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>dataUrl</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>chooseFriend</t>
+  </si>
+  <si>
     <t>用于字段值为array或者mixed操作，对其中的元素进行添加/删除/移动（使用edit，而不是update，防止混淆）
 fieldName:{from: eleArray中元素，原始位于哪个记录，如果没有（不是null或者undefined，而是没有key），说明是添加
  to: eleArray中元素，要移动到哪个记录，如果没有，说明是删除
  eleArray:要操作的记录。可以为空数组
 }</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>manipulateArray</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>captcha</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>sms</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>dataUrl</t>
-    <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -780,7 +808,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -816,10 +844,23 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1173,13 +1214,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O9"/>
+  <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="18.26953125" customWidth="1"/>
     <col min="2" max="2" width="45.36328125" customWidth="1"/>
@@ -1191,9 +1232,10 @@
     <col min="8" max="8" width="57.08984375" customWidth="1"/>
     <col min="9" max="9" width="54.36328125" customWidth="1"/>
     <col min="10" max="11" width="17.90625" customWidth="1"/>
+    <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1222,22 +1264,25 @@
         <v>7</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L1" t="s">
         <v>8</v>
       </c>
       <c r="M1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N1" t="s">
         <v>32</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="64" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="64" customHeight="1">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1275,7 +1320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="112" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="130.5">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -1298,7 +1343,7 @@
         <v>13</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>19</v>
@@ -1313,7 +1358,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="56.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" ht="70.5">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -1351,7 +1396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="42" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" ht="42">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -1389,7 +1434,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="143" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="143">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -1421,7 +1466,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" ht="105.75" customHeight="1">
       <c r="A9" s="6" t="s">
         <v>28</v>
       </c>
@@ -1449,7 +1494,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <sheetData/>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1463,7 +1508,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <sheetData/>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>